<commit_message>
Bagaimana dg aktivitas HIBAH?
</commit_message>
<xml_diff>
--- a/CoA SIKANGMAS.xlsx
+++ b/CoA SIKANGMAS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="110">
   <si>
     <t>Chart of Account</t>
   </si>
@@ -338,6 +338,12 @@
   </si>
   <si>
     <t>Tarik</t>
+  </si>
+  <si>
+    <t>Hibah</t>
+  </si>
+  <si>
+    <t>Implementasi dimana?</t>
   </si>
 </sst>
 </file>
@@ -345,12 +351,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -388,8 +394,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -405,7 +433,7 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -413,15 +441,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -436,10 +463,26 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -451,16 +494,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -474,23 +516,22 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -503,34 +544,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -541,19 +554,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -565,163 +608,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -833,6 +846,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -859,6 +896,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -877,45 +929,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -926,121 +939,121 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="11" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="14" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="13" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="13" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="10" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="10" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1049,29 +1062,29 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="13" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="14" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1151,6 +1164,24 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
@@ -1478,7 +1509,7 @@
   <dimension ref="A1:G83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
@@ -2534,29 +2565,95 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="4:4">
-      <c r="D77" s="27"/>
-    </row>
-    <row r="78" spans="4:4">
-      <c r="D78" s="27"/>
-    </row>
-    <row r="79" spans="4:4">
-      <c r="D79" s="27"/>
-    </row>
-    <row r="80" spans="4:4">
-      <c r="D80" s="27"/>
-    </row>
-    <row r="81" spans="4:4">
-      <c r="D81" s="27"/>
-    </row>
-    <row r="82" spans="4:4">
-      <c r="D82" s="27"/>
+    <row r="77" spans="1:5">
+      <c r="A77" s="27">
+        <v>19</v>
+      </c>
+      <c r="B77" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="C77" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="D77" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="E77" s="29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="27"/>
+      <c r="B78" s="31"/>
+      <c r="C78" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D78" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="E78" s="29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="27"/>
+      <c r="B79" s="31"/>
+      <c r="C79" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D79" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="E79" s="29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="27"/>
+      <c r="B80" s="31"/>
+      <c r="C80" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D80" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="E80" s="29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="27"/>
+      <c r="B81" s="31"/>
+      <c r="C81" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D81" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="E81" s="29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="27"/>
+      <c r="B82" s="31"/>
+      <c r="C82" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D82" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="E82" s="29" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="83" spans="4:4">
-      <c r="D83" s="27"/>
+      <c r="D83" s="33" t="s">
+        <v>109</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="33">
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="A4:A6"/>
@@ -2573,6 +2670,7 @@
     <mergeCell ref="A59:A68"/>
     <mergeCell ref="A70:A72"/>
     <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A77:A82"/>
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="B7:B11"/>
     <mergeCell ref="B12:B21"/>
@@ -2587,6 +2685,7 @@
     <mergeCell ref="B59:B68"/>
     <mergeCell ref="B70:B72"/>
     <mergeCell ref="B73:B74"/>
+    <mergeCell ref="B77:B82"/>
     <mergeCell ref="A1:E2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Done - Pembelian kredit, cicilan, peminjaman
</commit_message>
<xml_diff>
--- a/CoA SIKANGMAS.xlsx
+++ b/CoA SIKANGMAS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laravelVUESPA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26A1E85-443B-4BFE-A422-6FC96CFB04A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44B6EF0-9E10-4C93-989E-9357BD290C17}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="110">
   <si>
     <t>Chart of Account</t>
   </si>
@@ -512,7 +512,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -567,6 +567,33 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -585,32 +612,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -890,7 +893,7 @@
   <dimension ref="A1:G83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A65" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -902,20 +905,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
     </row>
     <row r="2" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="1:7" ht="30">
       <c r="A3" s="1" t="s">
@@ -938,10 +941,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="24">
+      <c r="A4" s="20">
         <v>1</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="23" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -955,8 +958,8 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="25"/>
-      <c r="B5" s="29"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="24"/>
       <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
@@ -968,8 +971,8 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="26"/>
-      <c r="B6" s="30"/>
+      <c r="A6" s="21"/>
+      <c r="B6" s="25"/>
       <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
@@ -981,10 +984,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="24">
+      <c r="A7" s="20">
         <v>2</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="23" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -998,8 +1001,8 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="25"/>
-      <c r="B8" s="29"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="24"/>
       <c r="C8" s="3" t="s">
         <v>19</v>
       </c>
@@ -1011,8 +1014,8 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="25"/>
-      <c r="B9" s="29"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="24"/>
       <c r="C9" s="3" t="s">
         <v>21</v>
       </c>
@@ -1024,8 +1027,8 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="25"/>
-      <c r="B10" s="29"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="24"/>
       <c r="C10" s="3" t="s">
         <v>23</v>
       </c>
@@ -1037,8 +1040,8 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="26"/>
-      <c r="B11" s="30"/>
+      <c r="A11" s="21"/>
+      <c r="B11" s="25"/>
       <c r="C11" s="3" t="s">
         <v>25</v>
       </c>
@@ -1050,21 +1053,21 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="24">
+      <c r="A12" s="20">
         <v>3</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="20"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="29"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="25"/>
-      <c r="B13" s="29"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="24"/>
       <c r="C13" s="3" t="s">
         <v>29</v>
       </c>
@@ -1074,8 +1077,8 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="25"/>
-      <c r="B14" s="29"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="24"/>
       <c r="C14" s="3" t="s">
         <v>31</v>
       </c>
@@ -1087,8 +1090,8 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="25"/>
-      <c r="B15" s="29"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="24"/>
       <c r="C15" s="3" t="s">
         <v>33</v>
       </c>
@@ -1100,17 +1103,17 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="27" customHeight="1">
-      <c r="A16" s="25"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="21" t="s">
+      <c r="A16" s="26"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="22"/>
-      <c r="E16" s="23"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="32"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="25"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="24"/>
       <c r="C17" s="3" t="s">
         <v>36</v>
       </c>
@@ -1122,8 +1125,8 @@
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="25"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="24"/>
       <c r="C18" s="3" t="s">
         <v>38</v>
       </c>
@@ -1135,8 +1138,8 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="25"/>
-      <c r="B19" s="29"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="24"/>
       <c r="C19" s="3" t="s">
         <v>40</v>
       </c>
@@ -1148,8 +1151,8 @@
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="25"/>
-      <c r="B20" s="29"/>
+      <c r="A20" s="26"/>
+      <c r="B20" s="24"/>
       <c r="C20" s="3" t="s">
         <v>42</v>
       </c>
@@ -1161,8 +1164,8 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="26"/>
-      <c r="B21" s="30"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="25"/>
       <c r="C21" s="3" t="s">
         <v>44</v>
       </c>
@@ -1174,10 +1177,10 @@
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="24">
+      <c r="A22" s="20">
         <v>4</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="20" t="s">
         <v>46</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -1191,8 +1194,8 @@
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="25"/>
-      <c r="B23" s="25"/>
+      <c r="A23" s="26"/>
+      <c r="B23" s="26"/>
       <c r="C23" s="3" t="s">
         <v>48</v>
       </c>
@@ -1204,8 +1207,8 @@
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="25"/>
-      <c r="B24" s="25"/>
+      <c r="A24" s="26"/>
+      <c r="B24" s="26"/>
       <c r="C24" s="3" t="s">
         <v>36</v>
       </c>
@@ -1217,8 +1220,8 @@
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="25"/>
-      <c r="B25" s="25"/>
+      <c r="A25" s="26"/>
+      <c r="B25" s="26"/>
       <c r="C25" s="3" t="s">
         <v>40</v>
       </c>
@@ -1230,8 +1233,8 @@
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="25"/>
-      <c r="B26" s="25"/>
+      <c r="A26" s="26"/>
+      <c r="B26" s="26"/>
       <c r="C26" s="3" t="s">
         <v>44</v>
       </c>
@@ -1243,10 +1246,10 @@
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="24">
+      <c r="A27" s="20">
         <v>5</v>
       </c>
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="23" t="s">
         <v>49</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -1260,8 +1263,8 @@
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="25"/>
-      <c r="B28" s="29"/>
+      <c r="A28" s="26"/>
+      <c r="B28" s="24"/>
       <c r="C28" s="3" t="s">
         <v>52</v>
       </c>
@@ -1273,8 +1276,8 @@
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="25"/>
-      <c r="B29" s="29"/>
+      <c r="A29" s="26"/>
+      <c r="B29" s="24"/>
       <c r="C29" s="3" t="s">
         <v>54</v>
       </c>
@@ -1286,8 +1289,8 @@
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="26"/>
-      <c r="B30" s="30"/>
+      <c r="A30" s="21"/>
+      <c r="B30" s="25"/>
       <c r="C30" s="3" t="s">
         <v>56</v>
       </c>
@@ -1314,10 +1317,10 @@
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="24">
+      <c r="A32" s="20">
         <v>7</v>
       </c>
-      <c r="B32" s="28" t="s">
+      <c r="B32" s="23" t="s">
         <v>60</v>
       </c>
       <c r="C32" s="3" t="s">
@@ -1331,8 +1334,8 @@
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="25"/>
-      <c r="B33" s="29"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="24"/>
       <c r="C33" s="3" t="s">
         <v>63</v>
       </c>
@@ -1344,8 +1347,8 @@
       </c>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="26"/>
-      <c r="B34" s="30"/>
+      <c r="A34" s="21"/>
+      <c r="B34" s="25"/>
       <c r="C34" s="3" t="s">
         <v>65</v>
       </c>
@@ -1357,10 +1360,10 @@
       </c>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="24">
+      <c r="A35" s="20">
         <v>8</v>
       </c>
-      <c r="B35" s="28" t="s">
+      <c r="B35" s="23" t="s">
         <v>67</v>
       </c>
       <c r="C35" s="3" t="s">
@@ -1374,8 +1377,8 @@
       </c>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="26"/>
-      <c r="B36" s="30"/>
+      <c r="A36" s="21"/>
+      <c r="B36" s="25"/>
       <c r="C36" s="3" t="s">
         <v>70</v>
       </c>
@@ -1387,10 +1390,10 @@
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="24">
+      <c r="A37" s="20">
         <v>9</v>
       </c>
-      <c r="B37" s="28" t="s">
+      <c r="B37" s="23" t="s">
         <v>72</v>
       </c>
       <c r="C37" s="3" t="s">
@@ -1404,8 +1407,8 @@
       </c>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="25"/>
-      <c r="B38" s="29"/>
+      <c r="A38" s="26"/>
+      <c r="B38" s="24"/>
       <c r="C38" s="3" t="s">
         <v>36</v>
       </c>
@@ -1417,8 +1420,8 @@
       </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="25"/>
-      <c r="B39" s="29"/>
+      <c r="A39" s="26"/>
+      <c r="B39" s="24"/>
       <c r="C39" s="3" t="s">
         <v>38</v>
       </c>
@@ -1430,8 +1433,8 @@
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="25"/>
-      <c r="B40" s="29"/>
+      <c r="A40" s="26"/>
+      <c r="B40" s="24"/>
       <c r="C40" s="3" t="s">
         <v>40</v>
       </c>
@@ -1443,8 +1446,8 @@
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="25"/>
-      <c r="B41" s="29"/>
+      <c r="A41" s="26"/>
+      <c r="B41" s="24"/>
       <c r="C41" s="3" t="s">
         <v>42</v>
       </c>
@@ -1456,8 +1459,8 @@
       </c>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="26"/>
-      <c r="B42" s="30"/>
+      <c r="A42" s="21"/>
+      <c r="B42" s="25"/>
       <c r="C42" s="3" t="s">
         <v>44</v>
       </c>
@@ -1469,10 +1472,10 @@
       </c>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="24">
-        <v>10</v>
-      </c>
-      <c r="B43" s="28" t="s">
+      <c r="A43" s="20">
+        <v>10</v>
+      </c>
+      <c r="B43" s="23" t="s">
         <v>75</v>
       </c>
       <c r="C43" s="3" t="s">
@@ -1486,8 +1489,8 @@
       </c>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="25"/>
-      <c r="B44" s="29"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="24"/>
       <c r="C44" s="3" t="s">
         <v>36</v>
       </c>
@@ -1499,8 +1502,8 @@
       </c>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="25"/>
-      <c r="B45" s="29"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="24"/>
       <c r="C45" s="3" t="s">
         <v>38</v>
       </c>
@@ -1512,8 +1515,8 @@
       </c>
     </row>
     <row r="46" spans="1:5">
-      <c r="A46" s="25"/>
-      <c r="B46" s="29"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="24"/>
       <c r="C46" s="3" t="s">
         <v>40</v>
       </c>
@@ -1525,8 +1528,8 @@
       </c>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="25"/>
-      <c r="B47" s="29"/>
+      <c r="A47" s="26"/>
+      <c r="B47" s="24"/>
       <c r="C47" s="3" t="s">
         <v>42</v>
       </c>
@@ -1538,8 +1541,8 @@
       </c>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="26"/>
-      <c r="B48" s="30"/>
+      <c r="A48" s="21"/>
+      <c r="B48" s="25"/>
       <c r="C48" s="3" t="s">
         <v>44</v>
       </c>
@@ -1551,10 +1554,10 @@
       </c>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="24">
+      <c r="A49" s="20">
         <v>11</v>
       </c>
-      <c r="B49" s="28" t="s">
+      <c r="B49" s="23" t="s">
         <v>76</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -1568,8 +1571,8 @@
       </c>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="25"/>
-      <c r="B50" s="29"/>
+      <c r="A50" s="26"/>
+      <c r="B50" s="24"/>
       <c r="C50" s="3" t="s">
         <v>36</v>
       </c>
@@ -1581,8 +1584,8 @@
       </c>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="25"/>
-      <c r="B51" s="29"/>
+      <c r="A51" s="26"/>
+      <c r="B51" s="24"/>
       <c r="C51" s="3" t="s">
         <v>38</v>
       </c>
@@ -1594,8 +1597,8 @@
       </c>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="25"/>
-      <c r="B52" s="29"/>
+      <c r="A52" s="26"/>
+      <c r="B52" s="24"/>
       <c r="C52" s="3" t="s">
         <v>40</v>
       </c>
@@ -1607,8 +1610,8 @@
       </c>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="25"/>
-      <c r="B53" s="29"/>
+      <c r="A53" s="26"/>
+      <c r="B53" s="24"/>
       <c r="C53" s="3" t="s">
         <v>42</v>
       </c>
@@ -1620,8 +1623,8 @@
       </c>
     </row>
     <row r="54" spans="1:5">
-      <c r="A54" s="26"/>
-      <c r="B54" s="30"/>
+      <c r="A54" s="21"/>
+      <c r="B54" s="25"/>
       <c r="C54" s="3" t="s">
         <v>44</v>
       </c>
@@ -1633,10 +1636,10 @@
       </c>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="24">
+      <c r="A55" s="20">
         <v>12</v>
       </c>
-      <c r="B55" s="28" t="s">
+      <c r="B55" s="23" t="s">
         <v>77</v>
       </c>
       <c r="C55" s="3" t="s">
@@ -1650,8 +1653,8 @@
       </c>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="25"/>
-      <c r="B56" s="29"/>
+      <c r="A56" s="26"/>
+      <c r="B56" s="24"/>
       <c r="C56" s="3" t="s">
         <v>36</v>
       </c>
@@ -1663,8 +1666,8 @@
       </c>
     </row>
     <row r="57" spans="1:5">
-      <c r="A57" s="25"/>
-      <c r="B57" s="29"/>
+      <c r="A57" s="26"/>
+      <c r="B57" s="24"/>
       <c r="C57" s="3" t="s">
         <v>40</v>
       </c>
@@ -1676,8 +1679,8 @@
       </c>
     </row>
     <row r="58" spans="1:5">
-      <c r="A58" s="26"/>
-      <c r="B58" s="30"/>
+      <c r="A58" s="21"/>
+      <c r="B58" s="25"/>
       <c r="C58" s="3" t="s">
         <v>44</v>
       </c>
@@ -1689,10 +1692,10 @@
       </c>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="24">
+      <c r="A59" s="20">
         <v>13</v>
       </c>
-      <c r="B59" s="28" t="s">
+      <c r="B59" s="23" t="s">
         <v>78</v>
       </c>
       <c r="C59" s="3" t="s">
@@ -1706,8 +1709,8 @@
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="25"/>
-      <c r="B60" s="29"/>
+      <c r="A60" s="26"/>
+      <c r="B60" s="24"/>
       <c r="C60" s="3" t="s">
         <v>81</v>
       </c>
@@ -1719,8 +1722,8 @@
       </c>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="25"/>
-      <c r="B61" s="29"/>
+      <c r="A61" s="26"/>
+      <c r="B61" s="24"/>
       <c r="C61" s="3" t="s">
         <v>83</v>
       </c>
@@ -1732,8 +1735,8 @@
       </c>
     </row>
     <row r="62" spans="1:5">
-      <c r="A62" s="25"/>
-      <c r="B62" s="29"/>
+      <c r="A62" s="26"/>
+      <c r="B62" s="24"/>
       <c r="C62" s="3" t="s">
         <v>85</v>
       </c>
@@ -1745,8 +1748,8 @@
       </c>
     </row>
     <row r="63" spans="1:5">
-      <c r="A63" s="25"/>
-      <c r="B63" s="29"/>
+      <c r="A63" s="26"/>
+      <c r="B63" s="24"/>
       <c r="C63" s="3" t="s">
         <v>87</v>
       </c>
@@ -1758,8 +1761,8 @@
       </c>
     </row>
     <row r="64" spans="1:5">
-      <c r="A64" s="25"/>
-      <c r="B64" s="29"/>
+      <c r="A64" s="26"/>
+      <c r="B64" s="24"/>
       <c r="C64" s="3" t="s">
         <v>89</v>
       </c>
@@ -1771,8 +1774,8 @@
       </c>
     </row>
     <row r="65" spans="1:5">
-      <c r="A65" s="25"/>
-      <c r="B65" s="29"/>
+      <c r="A65" s="26"/>
+      <c r="B65" s="24"/>
       <c r="C65" s="3" t="s">
         <v>91</v>
       </c>
@@ -1784,8 +1787,8 @@
       </c>
     </row>
     <row r="66" spans="1:5">
-      <c r="A66" s="25"/>
-      <c r="B66" s="29"/>
+      <c r="A66" s="26"/>
+      <c r="B66" s="24"/>
       <c r="C66" s="3" t="s">
         <v>93</v>
       </c>
@@ -1797,8 +1800,8 @@
       </c>
     </row>
     <row r="67" spans="1:5">
-      <c r="A67" s="25"/>
-      <c r="B67" s="29"/>
+      <c r="A67" s="26"/>
+      <c r="B67" s="24"/>
       <c r="C67" s="3" t="s">
         <v>95</v>
       </c>
@@ -1810,8 +1813,8 @@
       </c>
     </row>
     <row r="68" spans="1:5">
-      <c r="A68" s="26"/>
-      <c r="B68" s="30"/>
+      <c r="A68" s="21"/>
+      <c r="B68" s="25"/>
       <c r="C68" s="3" t="s">
         <v>97</v>
       </c>
@@ -1840,10 +1843,10 @@
       </c>
     </row>
     <row r="70" spans="1:5">
-      <c r="A70" s="24">
+      <c r="A70" s="20">
         <v>15</v>
       </c>
-      <c r="B70" s="28" t="s">
+      <c r="B70" s="23" t="s">
         <v>101</v>
       </c>
       <c r="C70" s="3" t="s">
@@ -1857,8 +1860,8 @@
       </c>
     </row>
     <row r="71" spans="1:5">
-      <c r="A71" s="25"/>
-      <c r="B71" s="29"/>
+      <c r="A71" s="26"/>
+      <c r="B71" s="24"/>
       <c r="C71" s="3" t="s">
         <v>36</v>
       </c>
@@ -1870,10 +1873,10 @@
       </c>
     </row>
     <row r="72" spans="1:5">
-      <c r="A72" s="26"/>
-      <c r="B72" s="30"/>
-      <c r="C72" s="3" t="s">
-        <v>38</v>
+      <c r="A72" s="21"/>
+      <c r="B72" s="25"/>
+      <c r="C72" s="33">
+        <v>8.7500000000000008E-2</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>103</v>
@@ -1883,10 +1886,10 @@
       </c>
     </row>
     <row r="73" spans="1:5">
-      <c r="A73" s="24">
+      <c r="A73" s="20">
         <v>16</v>
       </c>
-      <c r="B73" s="28" t="s">
+      <c r="B73" s="23" t="s">
         <v>104</v>
       </c>
       <c r="C73" s="3" t="s">
@@ -1900,10 +1903,10 @@
       </c>
     </row>
     <row r="74" spans="1:5">
-      <c r="A74" s="26"/>
-      <c r="B74" s="30"/>
-      <c r="C74" s="3" t="s">
-        <v>38</v>
+      <c r="A74" s="21"/>
+      <c r="B74" s="25"/>
+      <c r="C74" s="33">
+        <v>8.7500000000000008E-2</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>103</v>
@@ -1947,10 +1950,10 @@
       </c>
     </row>
     <row r="77" spans="1:5">
-      <c r="A77" s="27">
+      <c r="A77" s="22">
         <v>19</v>
       </c>
-      <c r="B77" s="31" t="s">
+      <c r="B77" s="18" t="s">
         <v>108</v>
       </c>
       <c r="C77" s="14" t="s">
@@ -1964,8 +1967,8 @@
       </c>
     </row>
     <row r="78" spans="1:5">
-      <c r="A78" s="27"/>
-      <c r="B78" s="31"/>
+      <c r="A78" s="22"/>
+      <c r="B78" s="18"/>
       <c r="C78" s="14" t="s">
         <v>36</v>
       </c>
@@ -1977,8 +1980,8 @@
       </c>
     </row>
     <row r="79" spans="1:5">
-      <c r="A79" s="27"/>
-      <c r="B79" s="31"/>
+      <c r="A79" s="22"/>
+      <c r="B79" s="18"/>
       <c r="C79" s="14" t="s">
         <v>38</v>
       </c>
@@ -1990,8 +1993,8 @@
       </c>
     </row>
     <row r="80" spans="1:5">
-      <c r="A80" s="27"/>
-      <c r="B80" s="31"/>
+      <c r="A80" s="22"/>
+      <c r="B80" s="18"/>
       <c r="C80" s="14" t="s">
         <v>40</v>
       </c>
@@ -2003,8 +2006,8 @@
       </c>
     </row>
     <row r="81" spans="1:5">
-      <c r="A81" s="27"/>
-      <c r="B81" s="31"/>
+      <c r="A81" s="22"/>
+      <c r="B81" s="18"/>
       <c r="C81" s="14" t="s">
         <v>42</v>
       </c>
@@ -2016,8 +2019,8 @@
       </c>
     </row>
     <row r="82" spans="1:5">
-      <c r="A82" s="27"/>
-      <c r="B82" s="31"/>
+      <c r="A82" s="22"/>
+      <c r="B82" s="18"/>
       <c r="C82" s="14" t="s">
         <v>44</v>
       </c>
@@ -2035,6 +2038,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A12:A21"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A37:A42"/>
+    <mergeCell ref="B70:B72"/>
+    <mergeCell ref="B73:B74"/>
+    <mergeCell ref="A43:A48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="A55:A58"/>
+    <mergeCell ref="A59:A68"/>
+    <mergeCell ref="A70:A72"/>
     <mergeCell ref="B77:B82"/>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="A73:A74"/>
@@ -2051,23 +2071,6 @@
     <mergeCell ref="B49:B54"/>
     <mergeCell ref="B55:B58"/>
     <mergeCell ref="B59:B68"/>
-    <mergeCell ref="B70:B72"/>
-    <mergeCell ref="B73:B74"/>
-    <mergeCell ref="A43:A48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="A55:A58"/>
-    <mergeCell ref="A59:A68"/>
-    <mergeCell ref="A70:A72"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A37:A42"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A12:A21"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>